<commit_message>
added definitions for solo referee mode
</commit_message>
<xml_diff>
--- a/diagrams/timekeeper/Timekeeper.xlsx
+++ b/diagrams/timekeeper/Timekeeper.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\owlcms-firmata\src\main\resources\devices\biy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\owlcms-firmata\diagrams\timekeeper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F7727C-3169-49FC-86ED-0C8259FB615F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D668E527-58AF-4F44-ABDC-502890774842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F9C8F068-60C0-4FDD-8C1E-880F519290ED}"/>
+    <workbookView xWindow="3840" yWindow="2805" windowWidth="21600" windowHeight="11295" xr2:uid="{F9C8F068-60C0-4FDD-8C1E-880F519290ED}"/>
   </bookViews>
   <sheets>
     <sheet name="TImekeeper" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
   <si>
     <t>pin</t>
   </si>
@@ -106,6 +106,36 @@
   </si>
   <si>
     <t>ignore A5</t>
+  </si>
+  <si>
+    <t>refbox/decision</t>
+  </si>
+  <si>
+    <t>Ref 1 simulated</t>
+  </si>
+  <si>
+    <t>1 good</t>
+  </si>
+  <si>
+    <t>Ref 2 simulated</t>
+  </si>
+  <si>
+    <t>Ref 3 simulated</t>
+  </si>
+  <si>
+    <t>2 good</t>
+  </si>
+  <si>
+    <t>3 good</t>
+  </si>
+  <si>
+    <t>1 bad</t>
+  </si>
+  <si>
+    <t>2 bad</t>
+  </si>
+  <si>
+    <t>3 bad</t>
   </si>
 </sst>
 </file>
@@ -491,7 +521,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -499,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{593FC154-758F-4104-A30E-11A530E91792}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,49 +647,151 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B6" s="4">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B7" s="4">
-        <v>15</v>
+        <v>7</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B8" s="4">
-        <v>16</v>
+        <v>7</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B9" s="4">
-        <v>17</v>
+        <v>8</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B10" s="4">
-        <v>18</v>
+        <v>8</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="4">
+        <v>8</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B17" s="4">
         <v>19</v>
       </c>
     </row>

</xml_diff>